<commit_message>
Modify label on plots in Energy_balance.ipynb
</commit_message>
<xml_diff>
--- a/FILES/BALANCE/Indicators.xlsx
+++ b/FILES/BALANCE/Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ehlimana\Documents\GitHub\Electricity-analysis\FILES\BALANCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38E30A7-C296-44C4-A0AA-DEB300FD3111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF36B60B-36A6-4C73-AF35-DE4F0D7ED517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9ECBF676-24DD-469E-AE51-5CD404D8790A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{9ECBF676-24DD-469E-AE51-5CD404D8790A}"/>
   </bookViews>
   <sheets>
     <sheet name="CO2 intensity of energy mix" sheetId="1" r:id="rId1"/>
@@ -185,12 +185,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1214,7 +1215,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A897B-69D8-4934-BE93-C910ADF1C8E7}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1469,7 +1472,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>2015</v>
       </c>
       <c r="B2">
@@ -1498,7 +1501,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2016</v>
       </c>
       <c r="B3">
@@ -1527,7 +1530,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>2017</v>
       </c>
       <c r="B4">
@@ -1556,7 +1559,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>2018</v>
       </c>
       <c r="B5">
@@ -1585,7 +1588,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>2019</v>
       </c>
       <c r="B6">
@@ -1614,7 +1617,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>2020</v>
       </c>
       <c r="B7">
@@ -1644,14 +1647,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D971DAA-37F5-4DFE-9177-B6849F822946}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1685,7 +1691,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>2015</v>
       </c>
       <c r="B2">
@@ -1714,7 +1720,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2016</v>
       </c>
       <c r="B3">
@@ -1743,7 +1749,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>2017</v>
       </c>
       <c r="B4">
@@ -1772,7 +1778,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>2018</v>
       </c>
       <c r="B5">
@@ -1801,7 +1807,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>2019</v>
       </c>
       <c r="B6">
@@ -1828,6 +1834,9 @@
       <c r="I6">
         <v>3.4</v>
       </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1836,10 +1845,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FE1C8C-39CD-43D2-8A11-9C91E0225AAA}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1877,7 +1886,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>2015</v>
       </c>
       <c r="B2">
@@ -1906,7 +1915,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2016</v>
       </c>
       <c r="B3">
@@ -1935,7 +1944,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>2017</v>
       </c>
       <c r="B4">
@@ -1964,7 +1973,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>2018</v>
       </c>
       <c r="B5">
@@ -1993,7 +2002,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>2019</v>
       </c>
       <c r="B6">
@@ -2020,6 +2029,9 @@
       <c r="I6">
         <v>148.19999999999999</v>
       </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2030,7 +2042,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202C0967-BCE8-4C73-8F68-60225B3EA382}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -2064,7 +2078,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>2015</v>
       </c>
       <c r="B2" s="2">
@@ -2093,7 +2107,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2016</v>
       </c>
       <c r="B3" s="2">
@@ -2122,7 +2136,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>2017</v>
       </c>
       <c r="B4" s="2">
@@ -2151,7 +2165,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>2018</v>
       </c>
       <c r="B5" s="2">
@@ -2180,7 +2194,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>2019</v>
       </c>
       <c r="B6" s="2">
@@ -2209,7 +2223,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>2020</v>
       </c>
       <c r="B7" s="2">

</xml_diff>